<commit_message>
Updated with EDA and work log
</commit_message>
<xml_diff>
--- a/personal-logs/ryan-koenig/WorkLog_rk.xlsx
+++ b/personal-logs/ryan-koenig/WorkLog_rk.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DataScience\Data599\w2020-data599-capstone-projects-ubc-udl\personal-logs\ryan-koenig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9DB5B0-089E-4488-A1BF-701C845D867D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C58D2AA-4742-4B61-83F7-024F2AC7DCAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="10" r:id="rId1"/>
     <sheet name="Week 2" sheetId="11" r:id="rId2"/>
+    <sheet name="Week 3" sheetId="12" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 1'!$A$1:$D$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Week 2'!$A$1:$D$57</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Week 3'!$A$1:$D$58</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="51">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -178,6 +180,18 @@
   </si>
   <si>
     <t>EDA Prep</t>
+  </si>
+  <si>
+    <t>Telegraf Finalizing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Documents </t>
+  </si>
+  <si>
+    <t>Telegraf Debugging</t>
+  </si>
+  <si>
+    <t>EDA Work</t>
   </si>
 </sst>
 </file>
@@ -946,7 +960,196 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="81">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2399,137 +2602,137 @@
     <mergeCell ref="A57:B57"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A15:C20 A30:C34 A22:C28">
-    <cfRule type="expression" dxfId="53" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="71" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="52" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B45">
-    <cfRule type="expression" dxfId="51" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C45">
-    <cfRule type="expression" dxfId="50" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="49" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C41">
-    <cfRule type="expression" dxfId="48" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="47" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B41">
-    <cfRule type="expression" dxfId="46" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C52">
-    <cfRule type="expression" dxfId="45" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C56">
-    <cfRule type="expression" dxfId="44" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B56 A47">
-    <cfRule type="expression" dxfId="43" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B52 A47">
-    <cfRule type="expression" dxfId="42" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B67">
-    <cfRule type="expression" dxfId="41" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B63">
-    <cfRule type="expression" dxfId="40" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C63">
-    <cfRule type="expression" dxfId="39" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C67">
-    <cfRule type="expression" dxfId="38" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="37" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B78">
-    <cfRule type="expression" dxfId="36" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C74">
-    <cfRule type="expression" dxfId="35" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C78">
-    <cfRule type="expression" dxfId="34" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B74">
-    <cfRule type="expression" dxfId="33" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="32" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="expression" dxfId="30" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="expression" dxfId="29" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2547,8 +2750,8 @@
   </sheetPr>
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView showGridLines="0" topLeftCell="A58" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2964,19 +3167,37 @@
       <c r="C47" s="31"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="18"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
+      <c r="A48" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="18"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="A49" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
+      <c r="A50" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
@@ -3014,7 +3235,7 @@
       <c r="C57" s="27"/>
       <c r="D57">
         <f>SUM(C48:C57)</f>
-        <v>0</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -3026,9 +3247,15 @@
       <c r="C58" s="31"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="18"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
+      <c r="A59" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
@@ -3076,7 +3303,7 @@
       <c r="C68" s="27"/>
       <c r="D68">
         <f>SUM(C59:C68)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -3088,9 +3315,15 @@
       <c r="C69" s="31"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="18"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
+      <c r="A70" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="25">
+        <v>5</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
@@ -3138,7 +3371,7 @@
       <c r="C79" s="27"/>
       <c r="D79">
         <f>SUM(C70:C79)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -3159,7 +3392,7 @@
       <c r="B82" s="17"/>
       <c r="C82" s="32">
         <f>SUM(C14:C79)</f>
-        <v>33.25</v>
+        <v>46.5</v>
       </c>
       <c r="D82" s="13"/>
     </row>
@@ -3212,136 +3445,876 @@
     <mergeCell ref="A58:B58"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A31:C35 A15:C21 A23:C29">
+    <cfRule type="expression" dxfId="53" priority="27" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="expression" dxfId="52" priority="26" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:B46">
+    <cfRule type="expression" dxfId="51" priority="23" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C46">
+    <cfRule type="expression" dxfId="50" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:C34">
+    <cfRule type="expression" dxfId="49" priority="24" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C42">
+    <cfRule type="expression" dxfId="48" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:B34">
+    <cfRule type="expression" dxfId="47" priority="25" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:B42">
+    <cfRule type="expression" dxfId="46" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C53">
+    <cfRule type="expression" dxfId="45" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48:C57">
+    <cfRule type="expression" dxfId="44" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49:B57 A48">
+    <cfRule type="expression" dxfId="43" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49:B53 A48">
+    <cfRule type="expression" dxfId="42" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:B68">
+    <cfRule type="expression" dxfId="41" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:B64">
+    <cfRule type="expression" dxfId="40" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:C64">
+    <cfRule type="expression" dxfId="39" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:C68">
+    <cfRule type="expression" dxfId="38" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47">
+    <cfRule type="expression" dxfId="37" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:B79">
+    <cfRule type="expression" dxfId="36" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70:C75">
+    <cfRule type="expression" dxfId="35" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C70:C79">
+    <cfRule type="expression" dxfId="34" priority="9" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A70:B75">
+    <cfRule type="expression" dxfId="33" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30">
+    <cfRule type="expression" dxfId="32" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="expression" dxfId="30" priority="4" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="expression" dxfId="29" priority="3" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B48">
+    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.25"/>
+  <pageSetup scale="99" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED696A20-CBEE-4FBB-BAA9-1EA57B348C85}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D91"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>44333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="33">
+        <f>D3</f>
+        <v>44333</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="20"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22">
+        <f>SUM(C15:C22)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="33">
+        <f>A14+1</f>
+        <v>44334</v>
+      </c>
+      <c r="B23" s="34"/>
+      <c r="C23" s="31"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="18"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="19"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30">
+        <f>SUM(C24:C30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="33">
+        <f>A23+1</f>
+        <v>44335</v>
+      </c>
+      <c r="B31" s="34"/>
+      <c r="C31" s="31"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="18"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="20"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36">
+        <f>SUM(C32:C36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="33">
+        <f>A31+1</f>
+        <v>44336</v>
+      </c>
+      <c r="B37" s="34"/>
+      <c r="C37" s="31"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="18"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="19"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="20"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="20"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="20"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47">
+        <f>SUM(C38:C47)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="33">
+        <f>A37+1</f>
+        <v>44337</v>
+      </c>
+      <c r="B48" s="34"/>
+      <c r="C48" s="31"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="18"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="18"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="18"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="18"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="18"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="19"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="20"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="20"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="20"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58">
+        <f>SUM(C49:C58)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="33">
+        <f>A48+1</f>
+        <v>44338</v>
+      </c>
+      <c r="B59" s="34"/>
+      <c r="C59" s="31"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="18"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="18"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="18"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="18"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="18"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="18"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="19"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="20"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="20"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="20"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69">
+        <f>SUM(C60:C69)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="33">
+        <f>A59+1</f>
+        <v>44339</v>
+      </c>
+      <c r="B70" s="34"/>
+      <c r="C70" s="31"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="18"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="18"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="18"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="18"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="18"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="18"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="19"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="26"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="20"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="27"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="20"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="20"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="27"/>
+      <c r="D80">
+        <f>SUM(C71:C80)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="10"/>
+      <c r="B82" s="28"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="12"/>
+    </row>
+    <row r="83" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="17"/>
+      <c r="C83" s="32">
+        <f>SUM(C14:C80)</f>
+        <v>9</v>
+      </c>
+      <c r="D83" s="13"/>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="9"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+    </row>
+    <row r="85" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A85" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="28"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="11"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="22"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="30"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="22"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="9"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="23"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+    </row>
+    <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A91" s="11"/>
+      <c r="B91" s="11"/>
+      <c r="C91" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A59:B59"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14 A32:C36 A24:C30 A15:C22">
     <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
+  <conditionalFormatting sqref="A23">
     <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B46">
+  <conditionalFormatting sqref="A38:B47">
     <cfRule type="expression" dxfId="24" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C46">
+  <conditionalFormatting sqref="C38:C47">
     <cfRule type="expression" dxfId="23" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:C34">
+  <conditionalFormatting sqref="C32:C35">
     <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C42">
+  <conditionalFormatting sqref="C38:C43">
     <cfRule type="expression" dxfId="21" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31:B34">
+  <conditionalFormatting sqref="A32:B35">
     <cfRule type="expression" dxfId="20" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B42">
+  <conditionalFormatting sqref="A38:B43">
     <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C53">
+  <conditionalFormatting sqref="C49:C54">
     <cfRule type="expression" dxfId="18" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48:C57">
+  <conditionalFormatting sqref="C49:C58">
     <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:B57 A48">
+  <conditionalFormatting sqref="A50:B58 A49">
     <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A49:B53 A48">
+  <conditionalFormatting sqref="A50:B54 A49">
     <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A59:B68">
+  <conditionalFormatting sqref="A60:B69">
     <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A59:B64">
+  <conditionalFormatting sqref="A60:B65">
     <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C64">
+  <conditionalFormatting sqref="C60:C65">
     <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C68">
+  <conditionalFormatting sqref="C60:C69">
     <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47">
+  <conditionalFormatting sqref="A48">
     <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70:B79">
+  <conditionalFormatting sqref="A71:B80">
     <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70:C75">
+  <conditionalFormatting sqref="C71:C76">
     <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70:C79">
+  <conditionalFormatting sqref="C71:C80">
     <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70:B75">
+  <conditionalFormatting sqref="A71:B76">
     <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30">
+  <conditionalFormatting sqref="A31">
     <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A36">
+  <conditionalFormatting sqref="A37">
     <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58">
+  <conditionalFormatting sqref="A59">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69">
+  <conditionalFormatting sqref="A70">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
+  <conditionalFormatting sqref="B49">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48">
+  <conditionalFormatting sqref="B49">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated log. Lost some previous days :/
</commit_message>
<xml_diff>
--- a/personal-logs/ryan-koenig/WorkLog_rk.xlsx
+++ b/personal-logs/ryan-koenig/WorkLog_rk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DataScience\Data599\w2020-data599-capstone-projects-ubc-udl\personal-logs\ryan-koenig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C58D2AA-4742-4B61-83F7-024F2AC7DCAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6023869C-9065-4584-B733-54C35121DE49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 1'!$A$1:$D$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Week 2'!$A$1:$D$57</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Week 3'!$A$1:$D$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Week 3'!$A$1:$D$59</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="61">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -192,6 +192,36 @@
   </si>
   <si>
     <t>EDA Work</t>
+  </si>
+  <si>
+    <t>Presentation Work</t>
+  </si>
+  <si>
+    <t>Interal morning meeting</t>
+  </si>
+  <si>
+    <t>Domain Expert Meeting</t>
+  </si>
+  <si>
+    <t>EWS Meeting</t>
+  </si>
+  <si>
+    <t>External Meeting</t>
+  </si>
+  <si>
+    <t>Presentation Prep</t>
+  </si>
+  <si>
+    <t>Week 3 Update Presentation</t>
+  </si>
+  <si>
+    <t>Anomaly Research</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Meeting with Scott</t>
   </si>
 </sst>
 </file>
@@ -1906,8 +1936,8 @@
   </sheetPr>
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A40" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -2750,8 +2780,8 @@
   </sheetPr>
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A58" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3591,10 +3621,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -3791,93 +3821,147 @@
       <c r="C23" s="31"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
+      <c r="A24" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
+      <c r="A26" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
+      <c r="A28" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30">
-        <f>SUM(C24:C30)</f>
-        <v>0</v>
+      <c r="A29" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="26">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="33">
+      <c r="A31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31">
+        <f>SUM(C24:C31)</f>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="33">
         <f>A23+1</f>
         <v>44335</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="31"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="31"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
+      <c r="A34" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="18"/>
       <c r="B35" s="25"/>
       <c r="C35" s="25"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="20"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36">
-        <f>SUM(C32:C36)</f>
-        <v>0</v>
-      </c>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="33">
-        <f>A31+1</f>
+      <c r="A37" s="20"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37">
+        <f>SUM(C33:C37)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="33">
+        <f>A32+1</f>
         <v>44336</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="31"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="31"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
@@ -3885,9 +3969,15 @@
       <c r="C39" s="25"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="18"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
+      <c r="A40" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
@@ -3905,103 +3995,133 @@
       <c r="C43" s="25"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="20"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="20"/>
       <c r="B46" s="27"/>
       <c r="C46" s="27"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="20"/>
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
-      <c r="D47">
-        <f>SUM(C38:C47)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="33">
-        <f>A37+1</f>
+      <c r="A48" s="20"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48">
+        <f>SUM(C39:C48)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="33">
+        <f>A38+1</f>
         <v>44337</v>
       </c>
-      <c r="B48" s="34"/>
-      <c r="C48" s="31"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="18"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="31"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
+      <c r="A50" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="25">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="18"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
+      <c r="A51" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
+      <c r="A52" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="18"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
+      <c r="A53" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
+      <c r="A54" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="19"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
+      <c r="A55" s="18"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="20"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="B57" s="27"/>
       <c r="C57" s="27"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="20"/>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
-      <c r="D58">
-        <f>SUM(C49:C58)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="33">
-        <f>A48+1</f>
+      <c r="A59" s="20"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59">
+        <f>SUM(C50:C59)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="33">
+        <f>A49+1</f>
         <v>44338</v>
       </c>
-      <c r="B59" s="34"/>
-      <c r="C59" s="31"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="31"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
@@ -4029,41 +4149,41 @@
       <c r="C65" s="25"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="19"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="26"/>
+      <c r="A66" s="18"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="20"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="20"/>
       <c r="B68" s="27"/>
       <c r="C68" s="27"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="20"/>
       <c r="B69" s="27"/>
       <c r="C69" s="27"/>
-      <c r="D69">
-        <f>SUM(C60:C69)</f>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="20"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="27"/>
+      <c r="D70">
+        <f>SUM(C61:C70)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="33">
-        <f>A59+1</f>
+    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="33">
+        <f>A60+1</f>
         <v>44339</v>
       </c>
-      <c r="B70" s="34"/>
-      <c r="C70" s="31"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="18"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="31"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
@@ -4091,14 +4211,14 @@
       <c r="C76" s="25"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="19"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="26"/>
+      <c r="A77" s="18"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="20"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
+      <c r="A78" s="19"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="20"/>
@@ -4109,50 +4229,50 @@
       <c r="A80" s="20"/>
       <c r="B80" s="27"/>
       <c r="C80" s="27"/>
-      <c r="D80">
-        <f>SUM(C71:C80)</f>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="20"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81">
+        <f>SUM(C72:C81)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="21"/>
-      <c r="B81" s="21"/>
-      <c r="C81" s="21"/>
-    </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="10"/>
-      <c r="B82" s="28"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="12"/>
-    </row>
-    <row r="83" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="17" t="s">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="10"/>
+      <c r="B83" s="28"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="12"/>
+    </row>
+    <row r="84" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B83" s="17"/>
-      <c r="C83" s="32">
-        <f>SUM(C14:C80)</f>
-        <v>9</v>
-      </c>
-      <c r="D83" s="13"/>
-    </row>
-    <row r="84" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="9"/>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
-    </row>
-    <row r="85" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A85" s="10" t="s">
+      <c r="B84" s="17"/>
+      <c r="C84" s="32">
+        <f>SUM(C14:C81)</f>
+        <v>24.75</v>
+      </c>
+      <c r="D84" s="13"/>
+    </row>
+    <row r="85" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="9"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+    </row>
+    <row r="86" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A86" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="28"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="11"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="22"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="30"/>
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="11"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="22"/>
@@ -4160,31 +4280,36 @@
       <c r="C87" s="30"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="9"/>
-      <c r="B88" s="29"/>
-      <c r="C88" s="29"/>
+      <c r="A88" s="22"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="30"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="23"/>
-      <c r="B89" s="23"/>
-      <c r="C89" s="23"/>
-    </row>
-    <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A91" s="11"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
+      <c r="A89" s="9"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="23"/>
+      <c r="B90" s="23"/>
+      <c r="C90" s="23"/>
+    </row>
+    <row r="92" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A92" s="11"/>
+      <c r="B92" s="11"/>
+      <c r="C92" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A60:B60"/>
   </mergeCells>
-  <conditionalFormatting sqref="A14 A32:C36 A24:C30 A15:C22">
+  <conditionalFormatting sqref="A14 A33:C37 A15:C22 A24:C31">
     <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
@@ -4194,127 +4319,127 @@
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B47">
+  <conditionalFormatting sqref="A39:B48">
     <cfRule type="expression" dxfId="24" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C47">
+  <conditionalFormatting sqref="C39:C48">
     <cfRule type="expression" dxfId="23" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C35">
+  <conditionalFormatting sqref="C33:C36">
     <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C43">
+  <conditionalFormatting sqref="C39:C44">
     <cfRule type="expression" dxfId="21" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A32:B35">
+  <conditionalFormatting sqref="A33:B36">
     <cfRule type="expression" dxfId="20" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B43">
+  <conditionalFormatting sqref="A39:B44">
     <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C54">
+  <conditionalFormatting sqref="C50:C55">
     <cfRule type="expression" dxfId="18" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C58">
+  <conditionalFormatting sqref="C50:C59">
     <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:B58 A49">
+  <conditionalFormatting sqref="A51:B59 A50">
     <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A50:B54 A49">
+  <conditionalFormatting sqref="A51:B55 A50">
     <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B69">
+  <conditionalFormatting sqref="A61:B70">
     <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B65">
+  <conditionalFormatting sqref="A61:B66">
     <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60:C65">
+  <conditionalFormatting sqref="C61:C66">
     <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60:C69">
+  <conditionalFormatting sqref="C61:C70">
     <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A48">
+  <conditionalFormatting sqref="A49">
     <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71:B80">
+  <conditionalFormatting sqref="A72:B81">
     <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71:C76">
+  <conditionalFormatting sqref="C72:C77">
     <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71:C80">
+  <conditionalFormatting sqref="C72:C81">
     <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71:B76">
+  <conditionalFormatting sqref="A72:B77">
     <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
+  <conditionalFormatting sqref="A32">
     <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+  <conditionalFormatting sqref="A38">
     <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
+  <conditionalFormatting sqref="A60">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70">
+  <conditionalFormatting sqref="A71">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
+  <conditionalFormatting sqref="B50">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
+  <conditionalFormatting sqref="B50">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
week 4 hours update
</commit_message>
<xml_diff>
--- a/personal-logs/ryan-koenig/WorkLog_rk.xlsx
+++ b/personal-logs/ryan-koenig/WorkLog_rk.xlsx
@@ -1,34 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\MDS\capstone\w2020-data599-capstone-projects-ubc-udl\personal-logs\ryan-koenig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DataScience\Data599\w2020-data599-capstone-projects-ubc-udl\personal-logs\ryan-koenig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E406EE1D-825C-4940-9BD8-B14AE418D916}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DD41E4-8982-4092-9922-F9E8836B1956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="10" r:id="rId1"/>
     <sheet name="Week 2" sheetId="11" r:id="rId2"/>
     <sheet name="Week 3" sheetId="12" r:id="rId3"/>
+    <sheet name="Week 4" sheetId="14" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 1'!$A$1:$D$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Week 2'!$A$1:$D$57</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Week 3'!$A$1:$D$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Week 4'!$A$1:$D$48</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="88">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -250,6 +263,48 @@
   </si>
   <si>
     <t>Download Data</t>
+  </si>
+  <si>
+    <t>Internal Morning Meeting</t>
+  </si>
+  <si>
+    <t>Data Cleaning Pipeline</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Internal Meeting Cover Pipeline</t>
+  </si>
+  <si>
+    <t>Week 4 Update Presentation</t>
+  </si>
+  <si>
+    <t>Inernal Morning Meeting</t>
+  </si>
+  <si>
+    <t>Data Cleaning -&gt; Training Pipeline</t>
+  </si>
+  <si>
+    <t>Dating Cleaning -&gt; Predict Pipeline</t>
+  </si>
+  <si>
+    <t>Model Evaluation on Dataset 5</t>
+  </si>
+  <si>
+    <t>Model Evaulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Meetings </t>
+  </si>
+  <si>
+    <t>Model Investigation</t>
+  </si>
+  <si>
+    <t>Model Evaluation</t>
+  </si>
+  <si>
+    <t>Notebook Adjusting</t>
   </si>
 </sst>
 </file>
@@ -257,7 +312,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -851,7 +906,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -962,7 +1017,7 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="20" borderId="19" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="20" borderId="19" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1018,7 +1073,196 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="104">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1940,15 +2184,15 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
@@ -1956,17 +2200,17 @@
       <c r="C1" s="8"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" s="2">
         <v>44319</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1976,7 +2220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1984,42 +2228,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
@@ -2031,7 +2275,7 @@
       </c>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="33">
         <f>D3</f>
         <v>44319</v>
@@ -2039,7 +2283,7 @@
       <c r="B14" s="34"/>
       <c r="C14" s="31"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>11</v>
       </c>
@@ -2050,7 +2294,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>12</v>
       </c>
@@ -2061,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>13</v>
       </c>
@@ -2072,7 +2316,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>14</v>
       </c>
@@ -2083,7 +2327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
@@ -2094,7 +2338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20"/>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -2103,7 +2347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="33">
         <f>A14+1</f>
         <v>44320</v>
@@ -2111,7 +2355,7 @@
       <c r="B21" s="34"/>
       <c r="C21" s="31"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>25</v>
       </c>
@@ -2122,7 +2366,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>18</v>
       </c>
@@ -2133,7 +2377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>26</v>
       </c>
@@ -2144,7 +2388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>19</v>
       </c>
@@ -2155,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>22</v>
       </c>
@@ -2166,7 +2410,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
         <v>26</v>
       </c>
@@ -2177,7 +2421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -2186,7 +2430,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="33">
         <f>A21+1</f>
         <v>44321</v>
@@ -2194,7 +2438,7 @@
       <c r="B29" s="34"/>
       <c r="C29" s="31"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>26</v>
       </c>
@@ -2205,7 +2449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>27</v>
       </c>
@@ -2216,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>13</v>
       </c>
@@ -2227,7 +2471,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>26</v>
       </c>
@@ -2238,7 +2482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="20"/>
       <c r="B34" s="27"/>
       <c r="C34" s="27"/>
@@ -2247,7 +2491,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="33">
         <f>A29+1</f>
         <v>44322</v>
@@ -2255,7 +2499,7 @@
       <c r="B35" s="34"/>
       <c r="C35" s="31"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>28</v>
       </c>
@@ -2266,7 +2510,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>29</v>
       </c>
@@ -2277,7 +2521,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
         <v>30</v>
       </c>
@@ -2288,7 +2532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>28</v>
       </c>
@@ -2299,7 +2543,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>31</v>
       </c>
@@ -2310,7 +2554,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>32</v>
       </c>
@@ -2321,7 +2565,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="19" t="s">
         <v>28</v>
       </c>
@@ -2332,17 +2576,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
     </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="20"/>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
@@ -2351,7 +2595,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="33">
         <f>A35+1</f>
         <v>44323</v>
@@ -2359,7 +2603,7 @@
       <c r="B46" s="34"/>
       <c r="C46" s="31"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
         <v>33</v>
       </c>
@@ -2370,47 +2614,47 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="18"/>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="18"/>
       <c r="B49" s="25"/>
       <c r="C49" s="25"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="18"/>
       <c r="B50" s="25"/>
       <c r="C50" s="25"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
       <c r="B51" s="25"/>
       <c r="C51" s="25"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="19"/>
       <c r="B53" s="26"/>
       <c r="C53" s="26"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="27"/>
       <c r="C54" s="27"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="20"/>
       <c r="B55" s="27"/>
       <c r="C55" s="27"/>
     </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="20"/>
       <c r="B56" s="27"/>
       <c r="C56" s="27"/>
@@ -2419,7 +2663,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="33">
         <f>A46+1</f>
         <v>44324</v>
@@ -2427,7 +2671,7 @@
       <c r="B57" s="34"/>
       <c r="C57" s="31"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
         <v>34</v>
       </c>
@@ -2438,47 +2682,47 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="25"/>
       <c r="C59" s="25"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
       <c r="B60" s="25"/>
       <c r="C60" s="25"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="25"/>
       <c r="C63" s="25"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="19"/>
       <c r="B64" s="26"/>
       <c r="C64" s="26"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="20"/>
       <c r="B65" s="27"/>
       <c r="C65" s="27"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="20"/>
       <c r="B66" s="27"/>
       <c r="C66" s="27"/>
     </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="20"/>
       <c r="B67" s="27"/>
       <c r="C67" s="27"/>
@@ -2487,7 +2731,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="33">
         <f>A57+1</f>
         <v>44325</v>
@@ -2495,7 +2739,7 @@
       <c r="B68" s="34"/>
       <c r="C68" s="31"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
         <v>33</v>
       </c>
@@ -2506,7 +2750,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
         <v>35</v>
       </c>
@@ -2517,42 +2761,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="25"/>
       <c r="C72" s="25"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="25"/>
       <c r="C73" s="25"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="18"/>
       <c r="B74" s="25"/>
       <c r="C74" s="25"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="19"/>
       <c r="B75" s="26"/>
       <c r="C75" s="26"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="20"/>
       <c r="B76" s="27"/>
       <c r="C76" s="27"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="20"/>
       <c r="B77" s="27"/>
       <c r="C77" s="27"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="20"/>
       <c r="B78" s="27"/>
       <c r="C78" s="27"/>
@@ -2561,18 +2805,18 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="10"/>
       <c r="B80" s="28"/>
       <c r="C80" s="28"/>
       <c r="D80" s="12"/>
     </row>
-    <row r="81" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
         <v>5</v>
       </c>
@@ -2583,12 +2827,12 @@
       </c>
       <c r="D81" s="13"/>
     </row>
-    <row r="82" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A82" s="9"/>
       <c r="B82" s="29"/>
       <c r="C82" s="29"/>
     </row>
-    <row r="83" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A83" s="10" t="s">
         <v>6</v>
       </c>
@@ -2596,27 +2840,27 @@
       <c r="C83" s="28"/>
       <c r="D83" s="11"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="22"/>
       <c r="B84" s="30"/>
       <c r="C84" s="30"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="22"/>
       <c r="B85" s="30"/>
       <c r="C85" s="30"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="9"/>
       <c r="B86" s="29"/>
       <c r="C86" s="29"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="23"/>
       <c r="B87" s="23"/>
       <c r="C87" s="23"/>
     </row>
-    <row r="89" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A89" s="11"/>
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
@@ -2632,137 +2876,137 @@
     <mergeCell ref="A57:B57"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A15:C20 A30:C34 A22:C28">
-    <cfRule type="expression" dxfId="76" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="71" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="75" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B45">
-    <cfRule type="expression" dxfId="74" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C45">
-    <cfRule type="expression" dxfId="73" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="72" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C41">
-    <cfRule type="expression" dxfId="71" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="70" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B41">
-    <cfRule type="expression" dxfId="69" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C52">
-    <cfRule type="expression" dxfId="68" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C56">
-    <cfRule type="expression" dxfId="67" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B56 A47">
-    <cfRule type="expression" dxfId="66" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B52 A47">
-    <cfRule type="expression" dxfId="65" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B67">
-    <cfRule type="expression" dxfId="64" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B63">
-    <cfRule type="expression" dxfId="63" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C63">
-    <cfRule type="expression" dxfId="62" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C67">
-    <cfRule type="expression" dxfId="61" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="60" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B78">
-    <cfRule type="expression" dxfId="59" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C74">
-    <cfRule type="expression" dxfId="58" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C78">
-    <cfRule type="expression" dxfId="57" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B74">
-    <cfRule type="expression" dxfId="56" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="55" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="54" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="expression" dxfId="53" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="expression" dxfId="52" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="50" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2784,15 +3028,15 @@
       <selection activeCell="C28" activeCellId="3" sqref="C20 C23 C26 C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
@@ -2800,17 +3044,17 @@
       <c r="C1" s="8"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" s="2">
         <v>44326</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2820,7 +3064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2828,42 +3072,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
@@ -2875,7 +3119,7 @@
       </c>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="33">
         <f>D3</f>
         <v>44326</v>
@@ -2883,7 +3127,7 @@
       <c r="B14" s="34"/>
       <c r="C14" s="31"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>36</v>
       </c>
@@ -2894,7 +3138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>37</v>
       </c>
@@ -2905,7 +3149,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>36</v>
       </c>
@@ -2916,7 +3160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>27</v>
       </c>
@@ -2927,7 +3171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>32</v>
       </c>
@@ -2938,7 +3182,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>38</v>
       </c>
@@ -2949,7 +3193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20"/>
       <c r="B21" s="27"/>
       <c r="C21" s="27"/>
@@ -2958,7 +3202,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="33">
         <f>A14+1</f>
         <v>44327</v>
@@ -2966,7 +3210,7 @@
       <c r="B22" s="34"/>
       <c r="C22" s="31"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>39</v>
       </c>
@@ -2977,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>40</v>
       </c>
@@ -2988,7 +3232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>37</v>
       </c>
@@ -2999,7 +3243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>41</v>
       </c>
@@ -3010,7 +3254,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>40</v>
       </c>
@@ -3021,7 +3265,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>42</v>
       </c>
@@ -3032,7 +3276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20"/>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -3041,7 +3285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="33">
         <f>A22+1</f>
         <v>44328</v>
@@ -3049,7 +3293,7 @@
       <c r="B30" s="34"/>
       <c r="C30" s="31"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>43</v>
       </c>
@@ -3060,7 +3304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>37</v>
       </c>
@@ -3071,7 +3315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>43</v>
       </c>
@@ -3082,12 +3326,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="18"/>
       <c r="B34" s="25"/>
       <c r="C34" s="25"/>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="20"/>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
@@ -3096,7 +3340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="33">
         <f>A30+1</f>
         <v>44329</v>
@@ -3104,7 +3348,7 @@
       <c r="B36" s="34"/>
       <c r="C36" s="31"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
         <v>44</v>
       </c>
@@ -3115,7 +3359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
         <v>37</v>
       </c>
@@ -3126,7 +3370,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>27</v>
       </c>
@@ -3137,7 +3381,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>42</v>
       </c>
@@ -3148,7 +3392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>42</v>
       </c>
@@ -3159,27 +3403,27 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="18"/>
       <c r="B42" s="25"/>
       <c r="C42" s="25"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="19"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="20"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="20"/>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
     </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="20"/>
       <c r="B46" s="27"/>
       <c r="C46" s="27"/>
@@ -3188,7 +3432,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="33">
         <f>A36+1</f>
         <v>44330</v>
@@ -3196,7 +3440,7 @@
       <c r="B47" s="34"/>
       <c r="C47" s="31"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
         <v>45</v>
       </c>
@@ -3207,7 +3451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
         <v>37</v>
       </c>
@@ -3218,7 +3462,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
         <v>44</v>
       </c>
@@ -3229,37 +3473,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="18"/>
       <c r="B51" s="25"/>
       <c r="C51" s="25"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="18"/>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="B53" s="25"/>
       <c r="C53" s="25"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="19"/>
       <c r="B54" s="26"/>
       <c r="C54" s="26"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="20"/>
       <c r="B55" s="27"/>
       <c r="C55" s="27"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="20"/>
       <c r="B56" s="27"/>
       <c r="C56" s="27"/>
     </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="20"/>
       <c r="B57" s="27"/>
       <c r="C57" s="27"/>
@@ -3268,7 +3512,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="33">
         <f>A47+1</f>
         <v>44331</v>
@@ -3276,7 +3520,7 @@
       <c r="B58" s="34"/>
       <c r="C58" s="31"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="18" t="s">
         <v>44</v>
       </c>
@@ -3287,47 +3531,47 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
       <c r="B60" s="25"/>
       <c r="C60" s="25"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="25"/>
       <c r="C63" s="25"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="18"/>
       <c r="B64" s="25"/>
       <c r="C64" s="25"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="19"/>
       <c r="B65" s="26"/>
       <c r="C65" s="26"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="20"/>
       <c r="B66" s="27"/>
       <c r="C66" s="27"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="20"/>
       <c r="B67" s="27"/>
       <c r="C67" s="27"/>
     </row>
-    <row r="68" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="20"/>
       <c r="B68" s="27"/>
       <c r="C68" s="27"/>
@@ -3336,7 +3580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="33">
         <f>A58+1</f>
         <v>44332</v>
@@ -3344,7 +3588,7 @@
       <c r="B69" s="34"/>
       <c r="C69" s="31"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
         <v>44</v>
       </c>
@@ -3355,47 +3599,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="25"/>
       <c r="C72" s="25"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="25"/>
       <c r="C73" s="25"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="18"/>
       <c r="B74" s="25"/>
       <c r="C74" s="25"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="18"/>
       <c r="B75" s="25"/>
       <c r="C75" s="25"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="19"/>
       <c r="B76" s="26"/>
       <c r="C76" s="26"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="20"/>
       <c r="B77" s="27"/>
       <c r="C77" s="27"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="20"/>
       <c r="B78" s="27"/>
       <c r="C78" s="27"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="20"/>
       <c r="B79" s="27"/>
       <c r="C79" s="27"/>
@@ -3404,18 +3648,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="21"/>
       <c r="B80" s="21"/>
       <c r="C80" s="21"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="10"/>
       <c r="B81" s="28"/>
       <c r="C81" s="28"/>
       <c r="D81" s="12"/>
     </row>
-    <row r="82" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>5</v>
       </c>
@@ -3426,12 +3670,12 @@
       </c>
       <c r="D82" s="13"/>
     </row>
-    <row r="83" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A83" s="9"/>
       <c r="B83" s="29"/>
       <c r="C83" s="29"/>
     </row>
-    <row r="84" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A84" s="10" t="s">
         <v>6</v>
       </c>
@@ -3439,27 +3683,27 @@
       <c r="C84" s="28"/>
       <c r="D84" s="11"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="22"/>
       <c r="B85" s="30"/>
       <c r="C85" s="30"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="22"/>
       <c r="B86" s="30"/>
       <c r="C86" s="30"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="9"/>
       <c r="B87" s="29"/>
       <c r="C87" s="29"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="23"/>
       <c r="B88" s="23"/>
       <c r="C88" s="23"/>
     </row>
-    <row r="90" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A90" s="11"/>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
@@ -3475,137 +3719,137 @@
     <mergeCell ref="A58:B58"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A31:C35 A15:C21 A23:C29">
-    <cfRule type="expression" dxfId="49" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="48" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="47" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="46" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C34">
-    <cfRule type="expression" dxfId="45" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="44" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B34">
-    <cfRule type="expression" dxfId="43" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="42" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="41" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="40" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B57 A48">
-    <cfRule type="expression" dxfId="39" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B53 A48">
-    <cfRule type="expression" dxfId="38" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="37" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="36" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="35" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="34" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="33" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="32" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="31" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="30" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="29" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="expression" dxfId="28" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="27" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="26" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="25" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="24" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="23" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3623,19 +3867,19 @@
   </sheetPr>
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView showGridLines="0" topLeftCell="A49" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
@@ -3643,17 +3887,17 @@
       <c r="C1" s="8"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D3" s="2">
         <v>44333</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -3663,7 +3907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3671,42 +3915,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
@@ -3718,7 +3962,7 @@
       </c>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="33">
         <f>D3</f>
         <v>44333</v>
@@ -3726,7 +3970,7 @@
       <c r="B14" s="34"/>
       <c r="C14" s="31"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>48</v>
       </c>
@@ -3737,7 +3981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>37</v>
       </c>
@@ -3748,7 +3992,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>48</v>
       </c>
@@ -3759,7 +4003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>27</v>
       </c>
@@ -3770,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>32</v>
       </c>
@@ -3781,7 +4025,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>48</v>
       </c>
@@ -3792,7 +4036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>47</v>
       </c>
@@ -3803,7 +4047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20"/>
       <c r="B22" s="27"/>
       <c r="C22" s="27"/>
@@ -3812,7 +4056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="33">
         <f>A14+1</f>
         <v>44334</v>
@@ -3820,7 +4064,7 @@
       <c r="B23" s="34"/>
       <c r="C23" s="31"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>48</v>
       </c>
@@ -3831,7 +4075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>54</v>
       </c>
@@ -3842,7 +4086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>52</v>
       </c>
@@ -3853,7 +4097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>37</v>
       </c>
@@ -3864,7 +4108,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>55</v>
       </c>
@@ -3875,7 +4119,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>47</v>
       </c>
@@ -3886,7 +4130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
         <v>56</v>
       </c>
@@ -3897,7 +4141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20"/>
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
@@ -3906,7 +4150,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="33">
         <f>A23+1</f>
         <v>44335</v>
@@ -3914,7 +4158,7 @@
       <c r="B32" s="34"/>
       <c r="C32" s="31"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>56</v>
       </c>
@@ -3925,7 +4169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
         <v>37</v>
       </c>
@@ -3936,7 +4180,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
         <v>56</v>
       </c>
@@ -3947,12 +4191,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="25"/>
       <c r="C36" s="25"/>
     </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20"/>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
@@ -3961,7 +4205,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="33">
         <f>A32+1</f>
         <v>44336</v>
@@ -3969,7 +4213,7 @@
       <c r="B38" s="34"/>
       <c r="C38" s="31"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
         <v>58</v>
       </c>
@@ -3980,7 +4224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>37</v>
       </c>
@@ -3991,7 +4235,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>61</v>
       </c>
@@ -4002,7 +4246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
         <v>59</v>
       </c>
@@ -4013,7 +4257,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
         <v>60</v>
       </c>
@@ -4024,7 +4268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="20"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
@@ -4033,7 +4277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="33">
         <f>A38+1</f>
         <v>44337</v>
@@ -4041,7 +4285,7 @@
       <c r="B45" s="34"/>
       <c r="C45" s="31"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="18" t="s">
         <v>49</v>
       </c>
@@ -4052,7 +4296,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
         <v>50</v>
       </c>
@@ -4063,7 +4307,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
         <v>51</v>
       </c>
@@ -4074,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
         <v>57</v>
       </c>
@@ -4085,7 +4329,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
         <v>33</v>
       </c>
@@ -4096,7 +4340,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
         <v>62</v>
       </c>
@@ -4107,22 +4351,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="19"/>
       <c r="B52" s="26"/>
       <c r="C52" s="26"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="20"/>
       <c r="B53" s="27"/>
       <c r="C53" s="27"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="20"/>
       <c r="B54" s="27"/>
       <c r="C54" s="27"/>
     </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="20"/>
       <c r="B55" s="27"/>
       <c r="C55" s="27"/>
@@ -4131,7 +4375,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="33">
         <f>A45+1</f>
         <v>44338</v>
@@ -4139,7 +4383,7 @@
       <c r="B56" s="34"/>
       <c r="C56" s="31"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="18" t="s">
         <v>63</v>
       </c>
@@ -4150,7 +4394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
         <v>64</v>
       </c>
@@ -4161,7 +4405,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="18" t="s">
         <v>63</v>
       </c>
@@ -4172,7 +4416,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
         <v>65</v>
       </c>
@@ -4183,32 +4427,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="19"/>
       <c r="B63" s="26"/>
       <c r="C63" s="26"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
       <c r="B64" s="27"/>
       <c r="C64" s="27"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="20"/>
       <c r="B65" s="27"/>
       <c r="C65" s="27"/>
     </row>
-    <row r="66" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="20"/>
       <c r="B66" s="27"/>
       <c r="C66" s="27"/>
@@ -4217,7 +4461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="33">
         <f>A56+1</f>
         <v>44339</v>
@@ -4225,7 +4469,7 @@
       <c r="B67" s="34"/>
       <c r="C67" s="31"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="18" t="s">
         <v>66</v>
       </c>
@@ -4236,47 +4480,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="18"/>
       <c r="B69" s="25"/>
       <c r="C69" s="25"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="18"/>
       <c r="B70" s="25"/>
       <c r="C70" s="25"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="18"/>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="18"/>
       <c r="B72" s="25"/>
       <c r="C72" s="25"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="18"/>
       <c r="B73" s="25"/>
       <c r="C73" s="25"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="19"/>
       <c r="B74" s="26"/>
       <c r="C74" s="26"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="20"/>
       <c r="B75" s="27"/>
       <c r="C75" s="27"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="20"/>
       <c r="B76" s="27"/>
       <c r="C76" s="27"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="20"/>
       <c r="B77" s="27"/>
       <c r="C77" s="27"/>
@@ -4285,18 +4529,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="21"/>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="10"/>
       <c r="B79" s="28"/>
       <c r="C79" s="28"/>
       <c r="D79" s="12"/>
     </row>
-    <row r="80" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
         <v>5</v>
       </c>
@@ -4307,12 +4551,12 @@
       </c>
       <c r="D80" s="13"/>
     </row>
-    <row r="81" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A81" s="9"/>
       <c r="B81" s="29"/>
       <c r="C81" s="29"/>
     </row>
-    <row r="82" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A82" s="10" t="s">
         <v>6</v>
       </c>
@@ -4320,27 +4564,27 @@
       <c r="C82" s="28"/>
       <c r="D82" s="11"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="22"/>
       <c r="B83" s="30"/>
       <c r="C83" s="30"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="22"/>
       <c r="B84" s="30"/>
       <c r="C84" s="30"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="9"/>
       <c r="B85" s="29"/>
       <c r="C85" s="29"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="23"/>
       <c r="B86" s="23"/>
       <c r="C86" s="23"/>
     </row>
-    <row r="88" spans="1:4" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A88" s="11"/>
       <c r="B88" s="11"/>
       <c r="C88" s="11"/>
@@ -4356,117 +4600,928 @@
     <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A33:C37 A15:C22 A39:C44 A24:C31">
-    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="21" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:C36">
-    <cfRule type="expression" dxfId="20" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B36">
-    <cfRule type="expression" dxfId="19" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C51">
-    <cfRule type="expression" dxfId="18" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C55">
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B55 A46">
+    <cfRule type="expression" dxfId="43" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47:B51 A46">
+    <cfRule type="expression" dxfId="42" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:B66">
+    <cfRule type="expression" dxfId="41" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:B62">
+    <cfRule type="expression" dxfId="40" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C62">
+    <cfRule type="expression" dxfId="39" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C66">
+    <cfRule type="expression" dxfId="38" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="expression" dxfId="37" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:B77">
+    <cfRule type="expression" dxfId="36" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C73">
+    <cfRule type="expression" dxfId="35" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C77">
+    <cfRule type="expression" dxfId="34" priority="9" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:B73">
+    <cfRule type="expression" dxfId="33" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="expression" dxfId="32" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="expression" dxfId="30" priority="4" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="expression" dxfId="29" priority="3" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46">
+    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.25"/>
+  <pageSetup scale="99" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57A58FC-2947-4579-97D9-2B4D6D1539A5}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D74"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>44340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="33">
+        <f>D3</f>
+        <v>44340</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:4" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20">
+        <f>SUM(C15:C20)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="33">
+        <f>A14+1</f>
+        <v>44341</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="31"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="20"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28">
+        <f>SUM(C22:C28)</f>
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="33">
+        <f>A21+1</f>
+        <v>44342</v>
+      </c>
+      <c r="B29" s="34"/>
+      <c r="C29" s="31"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="20"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34">
+        <f>SUM(C30:C34)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="33">
+        <f>A29+1</f>
+        <v>44343</v>
+      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="31"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="20"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41">
+        <f>SUM(C36:C41)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="33">
+        <f>A35+1</f>
+        <v>44344</v>
+      </c>
+      <c r="B42" s="34"/>
+      <c r="C42" s="31"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="20"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48">
+        <f>SUM(C43:C48)</f>
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="33">
+        <f>A42+1</f>
+        <v>44345</v>
+      </c>
+      <c r="B49" s="34"/>
+      <c r="C49" s="31"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="20"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="20"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55">
+        <f>SUM(C50:C55)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="33">
+        <f>A49+1</f>
+        <v>44346</v>
+      </c>
+      <c r="B56" s="34"/>
+      <c r="C56" s="31"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="20"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="20"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63">
+        <f>SUM(C57:C63)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="10"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="12"/>
+    </row>
+    <row r="66" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="17"/>
+      <c r="C66" s="32">
+        <f>SUM(C14:C63)</f>
+        <v>52.5</v>
+      </c>
+      <c r="D66" s="13"/>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="9"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+    </row>
+    <row r="68" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A68" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="11"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="22"/>
+      <c r="B69" s="30"/>
+      <c r="C69" s="30"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="22"/>
+      <c r="B70" s="30"/>
+      <c r="C70" s="30"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="9"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="23"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23"/>
+    </row>
+    <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A49:B49"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14 A34:C34 A41:C41 A19:C20 A28:C28 A48:C48 A54:C55 A62:C63">
+    <cfRule type="expression" dxfId="26" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="expression" dxfId="25" priority="42" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42">
+    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29">
+    <cfRule type="expression" dxfId="23" priority="27" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="expression" dxfId="22" priority="26" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56">
+    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:C33">
+    <cfRule type="expression" dxfId="19" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:C40">
+    <cfRule type="expression" dxfId="18" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:C18">
+    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:C27">
     <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A47:B51 A46">
+  <conditionalFormatting sqref="A30:C33">
     <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57:B66">
-    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57:B62">
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C62">
+  <conditionalFormatting sqref="A30:B33">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:C47">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:C47">
     <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C66">
-    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="10" priority="5" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:B77">
-    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68:C73">
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68:C77">
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:B73">
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38">
+  <conditionalFormatting sqref="A43 A44:B47">
+    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43 A44:B47">
+    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:B53">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:B53">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:C53">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:C53">
     <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A56">
+  <conditionalFormatting sqref="A57:B61">
     <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
+  <conditionalFormatting sqref="C57:C61">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C61">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A57:B61">
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated hours week 5
</commit_message>
<xml_diff>
--- a/personal-logs/ryan-koenig/WorkLog_rk.xlsx
+++ b/personal-logs/ryan-koenig/WorkLog_rk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DataScience\Data599\w2020-data599-capstone-projects-ubc-udl\personal-logs\ryan-koenig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C80A06C-079C-40EB-9A4A-18DD012966B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486EB240-8F53-43A7-9705-32C7CFE338E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="2250" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="99">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -1136,7 +1136,63 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="142">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3149,137 +3205,137 @@
     <mergeCell ref="A57:B57"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A15:C20 A30:C34 A22:C28">
-    <cfRule type="expression" dxfId="133" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="71" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="132" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B45">
-    <cfRule type="expression" dxfId="131" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C45">
-    <cfRule type="expression" dxfId="130" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="129" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C41">
-    <cfRule type="expression" dxfId="128" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="127" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B41">
-    <cfRule type="expression" dxfId="126" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C52">
-    <cfRule type="expression" dxfId="125" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C56">
-    <cfRule type="expression" dxfId="124" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B56 A47">
-    <cfRule type="expression" dxfId="123" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B52 A47">
-    <cfRule type="expression" dxfId="122" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B67">
-    <cfRule type="expression" dxfId="121" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B63">
-    <cfRule type="expression" dxfId="120" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C63">
-    <cfRule type="expression" dxfId="119" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C67">
-    <cfRule type="expression" dxfId="118" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="117" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B78">
-    <cfRule type="expression" dxfId="116" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C74">
-    <cfRule type="expression" dxfId="115" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C78">
-    <cfRule type="expression" dxfId="114" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B74">
-    <cfRule type="expression" dxfId="113" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="112" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="111" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="expression" dxfId="110" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="expression" dxfId="109" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="108" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="107" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3992,137 +4048,137 @@
     <mergeCell ref="A58:B58"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A31:C35 A15:C21 A23:C29">
-    <cfRule type="expression" dxfId="106" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="105" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="104" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="103" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C34">
-    <cfRule type="expression" dxfId="102" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="101" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B34">
-    <cfRule type="expression" dxfId="100" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="99" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="98" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="97" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B57 A48">
-    <cfRule type="expression" dxfId="96" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B53 A48">
-    <cfRule type="expression" dxfId="95" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="94" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="93" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="92" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="91" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="90" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="89" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="88" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="87" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="86" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="expression" dxfId="85" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="84" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="83" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="82" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="81" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="80" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4873,117 +4929,117 @@
     <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A33:C37 A15:C22 A39:C44 A24:C31">
-    <cfRule type="expression" dxfId="79" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="78" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:C36">
-    <cfRule type="expression" dxfId="77" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B36">
-    <cfRule type="expression" dxfId="76" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C51">
-    <cfRule type="expression" dxfId="75" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C55">
-    <cfRule type="expression" dxfId="74" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B55 A46">
-    <cfRule type="expression" dxfId="73" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B51 A46">
-    <cfRule type="expression" dxfId="72" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B66">
-    <cfRule type="expression" dxfId="71" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B62">
-    <cfRule type="expression" dxfId="70" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C62">
-    <cfRule type="expression" dxfId="69" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C66">
-    <cfRule type="expression" dxfId="68" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="67" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:B77">
-    <cfRule type="expression" dxfId="66" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C73">
-    <cfRule type="expression" dxfId="65" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C77">
-    <cfRule type="expression" dxfId="64" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:B73">
-    <cfRule type="expression" dxfId="63" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="62" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="expression" dxfId="61" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" dxfId="60" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="expression" dxfId="59" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="58" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="57" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5664,137 +5720,137 @@
     <mergeCell ref="A49:B49"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A34:C34 A41:C41 A19:C20 A28:C28 A48:C48 A54:C55 A62:C63">
-    <cfRule type="expression" dxfId="56" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="55" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="54" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="53" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="52" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="expression" dxfId="51" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" dxfId="50" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="49" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:C40">
-    <cfRule type="expression" dxfId="48" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:C18">
-    <cfRule type="expression" dxfId="47" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:C27">
-    <cfRule type="expression" dxfId="46" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:C33">
-    <cfRule type="expression" dxfId="45" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="44" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C47">
-    <cfRule type="expression" dxfId="43" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C47">
-    <cfRule type="expression" dxfId="42" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43 A44:B47">
-    <cfRule type="expression" dxfId="41" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43 A44:B47">
-    <cfRule type="expression" dxfId="40" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="39" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="38" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B53">
-    <cfRule type="expression" dxfId="37" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B53">
-    <cfRule type="expression" dxfId="36" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C53">
-    <cfRule type="expression" dxfId="35" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C53">
-    <cfRule type="expression" dxfId="34" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B61">
-    <cfRule type="expression" dxfId="33" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C61">
-    <cfRule type="expression" dxfId="32" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C61">
-    <cfRule type="expression" dxfId="31" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B61">
-    <cfRule type="expression" dxfId="30" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5812,8 +5868,8 @@
   </sheetPr>
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -6362,9 +6418,15 @@
       <c r="C59" s="31"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+      <c r="A60" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="18"/>
@@ -6392,7 +6454,7 @@
       <c r="C65" s="27"/>
       <c r="D65">
         <f>SUM(C60:C65)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -6404,9 +6466,15 @@
       <c r="C66" s="31"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
+      <c r="A67" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B67" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="18"/>
@@ -6439,7 +6507,7 @@
       <c r="C73" s="27"/>
       <c r="D73">
         <f>SUM(C67:C73)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -6460,7 +6528,7 @@
       <c r="B76" s="17"/>
       <c r="C76" s="32">
         <f>SUM(C14:C73)</f>
-        <v>37.75</v>
+        <v>41.75</v>
       </c>
       <c r="D76" s="13"/>
     </row>
@@ -6513,151 +6581,191 @@
     <mergeCell ref="A59:B59"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A40:C40 A20:C25 A33:C33 A58:C58 A64:C65 A72:C73 A42:C50">
-    <cfRule type="expression" dxfId="29" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
+    <cfRule type="expression" dxfId="34" priority="37" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="expression" dxfId="33" priority="36" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="expression" dxfId="31" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C39">
+    <cfRule type="expression" dxfId="30" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:C19">
+    <cfRule type="expression" dxfId="29" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:C32">
+    <cfRule type="expression" dxfId="28" priority="31" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:C39">
+    <cfRule type="expression" dxfId="27" priority="30" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:B39">
     <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="expression" dxfId="25" priority="28" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35:C39">
-    <cfRule type="expression" dxfId="22" priority="20" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:C19">
-    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:C32">
-    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:C39">
-    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:B39">
-    <cfRule type="expression" dxfId="18" priority="21" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C52:C55 C57">
-    <cfRule type="expression" dxfId="17" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C55 C57">
-    <cfRule type="expression" dxfId="16" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52 A53:B55 A57:B57">
-    <cfRule type="expression" dxfId="15" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52 A53:B55 A57:B57">
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B63">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B63">
+    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61:C63">
+    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61:C63">
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:B71">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C71">
+    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C71">
     <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B63">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B63">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60:C63">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60:C63">
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:B71">
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67:C71">
-    <cfRule type="expression" dxfId="6" priority="5" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67:C71">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:B71">
+  <conditionalFormatting sqref="A68:B71">
+    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B56">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B56">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B60">
+    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B60">
     <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C67">
     <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C67">
     <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B56">
+  <conditionalFormatting sqref="A67:B67">
     <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B56">
+  <conditionalFormatting sqref="A67:B67">
     <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated hours week 6
</commit_message>
<xml_diff>
--- a/personal-logs/ryan-koenig/WorkLog_rk.xlsx
+++ b/personal-logs/ryan-koenig/WorkLog_rk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DataScience\Data599\w2020-data599-capstone-projects-ubc-udl\personal-logs\ryan-koenig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486EB240-8F53-43A7-9705-32C7CFE338E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C947D4ED-9838-4979-A92C-B4D29E01E083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2250" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="10" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Week 3" sheetId="12" r:id="rId3"/>
     <sheet name="Week 4" sheetId="14" r:id="rId4"/>
     <sheet name="Week 5" sheetId="16" r:id="rId5"/>
+    <sheet name="Week 6" sheetId="17" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 1'!$A$1:$D$56</definedName>
@@ -25,6 +26,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Week 3'!$A$1:$D$55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Week 4'!$A$1:$D$48</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Week 5'!$A$1:$D$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Week 6'!$A$1:$D$56</definedName>
     <definedName name="valuevx">42.314159</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="104">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -340,6 +342,21 @@
   </si>
   <si>
     <t>Model Parameter Evaluation</t>
+  </si>
+  <si>
+    <t>Threshold Rule Investigation</t>
+  </si>
+  <si>
+    <t>Week 6 Update Presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal Meeting </t>
+  </si>
+  <si>
+    <t>Appendix C Results</t>
+  </si>
+  <si>
+    <t>Appendix C Figures</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1153,448 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="142">
+  <dxfs count="205">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3205,137 +3663,137 @@
     <mergeCell ref="A57:B57"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A15:C20 A30:C34 A22:C28">
-    <cfRule type="expression" dxfId="141" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="204" priority="71" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="140" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B45">
-    <cfRule type="expression" dxfId="139" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C45">
-    <cfRule type="expression" dxfId="138" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="137" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="200" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C41">
-    <cfRule type="expression" dxfId="136" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="135" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B41">
-    <cfRule type="expression" dxfId="134" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="197" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C52">
-    <cfRule type="expression" dxfId="133" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="196" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C56">
-    <cfRule type="expression" dxfId="132" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="195" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B56 A47">
-    <cfRule type="expression" dxfId="131" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="194" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B52 A47">
-    <cfRule type="expression" dxfId="130" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="193" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B67">
-    <cfRule type="expression" dxfId="129" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="192" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B63">
-    <cfRule type="expression" dxfId="128" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="191" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C63">
-    <cfRule type="expression" dxfId="127" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="190" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C67">
-    <cfRule type="expression" dxfId="126" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="189" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="125" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B78">
-    <cfRule type="expression" dxfId="124" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C74">
-    <cfRule type="expression" dxfId="123" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C78">
-    <cfRule type="expression" dxfId="122" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B74">
-    <cfRule type="expression" dxfId="121" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="120" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="119" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="expression" dxfId="118" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="expression" dxfId="117" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="116" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="115" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4048,137 +4506,137 @@
     <mergeCell ref="A58:B58"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A31:C35 A15:C21 A23:C29">
-    <cfRule type="expression" dxfId="114" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="113" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="112" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="111" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C34">
-    <cfRule type="expression" dxfId="110" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="109" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B34">
-    <cfRule type="expression" dxfId="108" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="107" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="106" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="105" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B57 A48">
-    <cfRule type="expression" dxfId="104" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B53 A48">
-    <cfRule type="expression" dxfId="103" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="102" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="101" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="100" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="99" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="98" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="97" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="96" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="95" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="94" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="expression" dxfId="93" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="92" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="91" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="90" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="89" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="88" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4929,117 +5387,117 @@
     <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A33:C37 A15:C22 A39:C44 A24:C31">
-    <cfRule type="expression" dxfId="87" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="86" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:C36">
-    <cfRule type="expression" dxfId="85" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B36">
-    <cfRule type="expression" dxfId="84" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C51">
-    <cfRule type="expression" dxfId="83" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C55">
-    <cfRule type="expression" dxfId="82" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B55 A46">
-    <cfRule type="expression" dxfId="81" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B51 A46">
-    <cfRule type="expression" dxfId="80" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B66">
-    <cfRule type="expression" dxfId="79" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B62">
-    <cfRule type="expression" dxfId="78" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C62">
-    <cfRule type="expression" dxfId="77" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C66">
-    <cfRule type="expression" dxfId="76" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="75" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:B77">
-    <cfRule type="expression" dxfId="74" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C73">
-    <cfRule type="expression" dxfId="73" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C77">
-    <cfRule type="expression" dxfId="72" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:B73">
-    <cfRule type="expression" dxfId="71" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="70" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="expression" dxfId="69" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" dxfId="68" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="expression" dxfId="67" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="65" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5057,8 +5515,8 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -5720,137 +6178,137 @@
     <mergeCell ref="A49:B49"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A34:C34 A41:C41 A19:C20 A28:C28 A48:C48 A54:C55 A62:C63">
-    <cfRule type="expression" dxfId="64" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="63" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="62" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="61" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="60" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="expression" dxfId="59" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" dxfId="58" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="57" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:C40">
-    <cfRule type="expression" dxfId="56" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:C18">
-    <cfRule type="expression" dxfId="55" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:C27">
-    <cfRule type="expression" dxfId="54" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:C33">
-    <cfRule type="expression" dxfId="53" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="52" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C47">
-    <cfRule type="expression" dxfId="51" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C47">
-    <cfRule type="expression" dxfId="50" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43 A44:B47">
-    <cfRule type="expression" dxfId="49" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43 A44:B47">
-    <cfRule type="expression" dxfId="48" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="47" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="46" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B53">
-    <cfRule type="expression" dxfId="45" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B53">
-    <cfRule type="expression" dxfId="44" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C53">
-    <cfRule type="expression" dxfId="43" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C53">
-    <cfRule type="expression" dxfId="42" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B61">
-    <cfRule type="expression" dxfId="41" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C61">
-    <cfRule type="expression" dxfId="40" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C61">
-    <cfRule type="expression" dxfId="39" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B61">
-    <cfRule type="expression" dxfId="38" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5868,7 +6326,7 @@
   </sheetPr>
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
@@ -6581,192 +7039,1129 @@
     <mergeCell ref="A59:B59"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A40:C40 A20:C25 A33:C33 A58:C58 A64:C65 A72:C73 A42:C50">
-    <cfRule type="expression" dxfId="37" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="expression" dxfId="35" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
+    <cfRule type="expression" dxfId="97" priority="37" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
+    <cfRule type="expression" dxfId="96" priority="36" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="expression" dxfId="95" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="expression" dxfId="94" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C39">
+    <cfRule type="expression" dxfId="93" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15:C19">
+    <cfRule type="expression" dxfId="92" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:C32">
+    <cfRule type="expression" dxfId="91" priority="31" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:C39">
+    <cfRule type="expression" dxfId="90" priority="30" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:B39">
+    <cfRule type="expression" dxfId="89" priority="29" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:C55 C57">
+    <cfRule type="expression" dxfId="88" priority="23" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:C55 C57">
+    <cfRule type="expression" dxfId="87" priority="24" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52 A53:B55 A57:B57">
+    <cfRule type="expression" dxfId="86" priority="26" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52 A53:B55 A57:B57">
+    <cfRule type="expression" dxfId="85" priority="25" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="84" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="83" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B63">
+    <cfRule type="expression" dxfId="82" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B63">
+    <cfRule type="expression" dxfId="81" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61:C63">
+    <cfRule type="expression" dxfId="80" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61:C63">
+    <cfRule type="expression" dxfId="79" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:B71">
+    <cfRule type="expression" dxfId="78" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C71">
+    <cfRule type="expression" dxfId="77" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C71">
+    <cfRule type="expression" dxfId="76" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:B71">
+    <cfRule type="expression" dxfId="75" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="74" priority="9" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="expression" dxfId="73" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B56">
+    <cfRule type="expression" dxfId="72" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B56">
+    <cfRule type="expression" dxfId="71" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="70" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="69" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B60">
+    <cfRule type="expression" dxfId="68" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B60">
+    <cfRule type="expression" dxfId="67" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" dxfId="66" priority="1" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
+    <cfRule type="expression" dxfId="65" priority="2" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:B67">
+    <cfRule type="expression" dxfId="64" priority="4" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67:B67">
+    <cfRule type="expression" dxfId="63" priority="3" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.25"/>
+  <pageSetup scale="99" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BFA658-CC50-40EB-827B-912471ABC0D9}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D82"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="2">
+        <v>44354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="35">
+        <f>D3</f>
+        <v>44354</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+    </row>
+    <row r="24" spans="1:4" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="20"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24">
+        <f>SUM(C15:C24)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="35">
+        <f>A14+1</f>
+        <v>44355</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="18"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="20"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32">
+        <f>SUM(C26:C32)</f>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="35">
+        <f>A25+1</f>
+        <v>44356</v>
+      </c>
+      <c r="B33" s="36"/>
+      <c r="C33" s="31"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="18"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="18"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="20"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39">
+        <f>SUM(C34:C39)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="35">
+        <f>A33+1</f>
+        <v>44357</v>
+      </c>
+      <c r="B40" s="36"/>
+      <c r="C40" s="31"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="25"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="25"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="20"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48">
+        <f>SUM(C41:C48)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="35">
+        <f>A40+1</f>
+        <v>44358</v>
+      </c>
+      <c r="B49" s="36"/>
+      <c r="C49" s="31"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="18"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="18"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="18"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="20"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56">
+        <f>SUM(C50:C56)</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="35">
+        <f>A49+1</f>
+        <v>44359</v>
+      </c>
+      <c r="B57" s="36"/>
+      <c r="C57" s="31"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="18"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="18"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="18"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="18"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="20"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="20"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63">
+        <f>SUM(C58:C63)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="35">
+        <f>A57+1</f>
+        <v>44360</v>
+      </c>
+      <c r="B64" s="36"/>
+      <c r="C64" s="31"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="18"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="18"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="18"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="18"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="20"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="27"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="20"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="27"/>
+      <c r="D71">
+        <f>SUM(C65:C71)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="10"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="12"/>
+    </row>
+    <row r="74" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="17"/>
+      <c r="C74" s="32">
+        <f>SUM(C14:C71)</f>
+        <v>40.25</v>
+      </c>
+      <c r="D74" s="13"/>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="9"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+    </row>
+    <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A76" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="28"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="11"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="22"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="22"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="30"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="9"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="23"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+    </row>
+    <row r="82" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A57:B57"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A14 A39:C39 A32:C32 A56:C56 A62:C63 A70:C71 A42:C42 A16:C24 A44:C44 A46:C48">
+    <cfRule type="expression" dxfId="62" priority="64" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25">
+    <cfRule type="expression" dxfId="61" priority="63" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="expression" dxfId="60" priority="60" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="expression" dxfId="59" priority="62" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40">
+    <cfRule type="expression" dxfId="58" priority="61" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="expression" dxfId="57" priority="59" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="expression" dxfId="56" priority="58" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:C38">
+    <cfRule type="expression" dxfId="55" priority="53" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:C31">
+    <cfRule type="expression" dxfId="54" priority="56" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:C38">
+    <cfRule type="expression" dxfId="53" priority="55" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:B38">
+    <cfRule type="expression" dxfId="52" priority="54" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:C51 C55 C53">
+    <cfRule type="expression" dxfId="51" priority="49" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:C51 C55 C53">
+    <cfRule type="expression" dxfId="50" priority="50" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50 A51:B51 A55:B55 A53:B53">
+    <cfRule type="expression" dxfId="49" priority="52" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50 A51:B51 A55:B55 A53:B53">
+    <cfRule type="expression" dxfId="48" priority="51" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:B61">
+    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:B61">
+    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:C61">
+    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:C61">
+    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66:B69">
+    <cfRule type="expression" dxfId="41" priority="42" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66:C69">
+    <cfRule type="expression" dxfId="40" priority="39" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66:C69">
+    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66:B69">
+    <cfRule type="expression" dxfId="38" priority="41" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="37" priority="35" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="36" priority="36" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B54">
+    <cfRule type="expression" dxfId="35" priority="38" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B54">
     <cfRule type="expression" dxfId="34" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41">
-    <cfRule type="expression" dxfId="33" priority="36" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="expression" dxfId="31" priority="33" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35:C39">
-    <cfRule type="expression" dxfId="30" priority="28" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15:C19">
-    <cfRule type="expression" dxfId="29" priority="32" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:C32">
-    <cfRule type="expression" dxfId="28" priority="31" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:C39">
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="33" priority="31" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="32" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58:B58">
+    <cfRule type="expression" dxfId="31" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58:B58">
+    <cfRule type="expression" dxfId="30" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="29" priority="27" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="28" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65:B65">
     <cfRule type="expression" dxfId="27" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35:B39">
+  <conditionalFormatting sqref="A65:B65">
     <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52:C55 C57">
+  <conditionalFormatting sqref="C15">
     <cfRule type="expression" dxfId="25" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52:C55 C57">
+  <conditionalFormatting sqref="C15">
     <cfRule type="expression" dxfId="24" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52 A53:B55 A57:B57">
+  <conditionalFormatting sqref="A15:B15">
     <cfRule type="expression" dxfId="23" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52 A53:B55 A57:B57">
+  <conditionalFormatting sqref="A15:B15">
     <cfRule type="expression" dxfId="22" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A26:C26">
+    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:C27">
+    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:C29">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:C28">
+    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:C30">
+    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:C41">
+    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:B41">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" dxfId="13" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:C43">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:B43">
+    <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" dxfId="10" priority="9" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:C45">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:B45">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B63">
-    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B63">
-    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61:C63">
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61:C63">
-    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:B71">
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68:C71">
-    <cfRule type="expression" dxfId="14" priority="13" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68:C71">
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A68:B71">
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B56">
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B56">
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B60">
-    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B60">
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:B67">
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:B67">
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
hours for week 7
</commit_message>
<xml_diff>
--- a/personal-logs/ryan-koenig/WorkLog_rk.xlsx
+++ b/personal-logs/ryan-koenig/WorkLog_rk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\DataScience\Data599\w2020-data599-capstone-projects-ubc-udl\personal-logs\ryan-koenig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C6BDC9-BC23-4D75-8790-B4EAFD340CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1706EC5D-812E-44E7-B049-EC54520EEFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="114">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -370,13 +370,25 @@
     <t>Code Package Review</t>
   </si>
   <si>
-    <t>Review</t>
-  </si>
-  <si>
     <t>Figure Creation / Results</t>
   </si>
   <si>
     <t>UBC Meeting</t>
+  </si>
+  <si>
+    <t>Results folder cleanup</t>
+  </si>
+  <si>
+    <t>Demo notebook review</t>
+  </si>
+  <si>
+    <t>Code Review</t>
+  </si>
+  <si>
+    <t>Demo notebook Investigation</t>
+  </si>
+  <si>
+    <t>Demo notebook Cleanup</t>
   </si>
 </sst>
 </file>
@@ -680,7 +692,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -953,6 +965,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1000,7 +1025,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1126,6 +1151,10 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1173,7 +1202,434 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="269">
+  <dxfs count="330">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4131,137 +4587,137 @@
     <mergeCell ref="A57:B57"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A15:C20 A30:C34 A22:C28">
-    <cfRule type="expression" dxfId="268" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="324" priority="71" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="267" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="323" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B45">
-    <cfRule type="expression" dxfId="266" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="322" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C45">
-    <cfRule type="expression" dxfId="265" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="321" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="264" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="320" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C41">
-    <cfRule type="expression" dxfId="263" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="319" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="262" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="318" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B41">
-    <cfRule type="expression" dxfId="261" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="317" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C52">
-    <cfRule type="expression" dxfId="260" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="316" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:C56">
-    <cfRule type="expression" dxfId="259" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="315" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B56 A47">
-    <cfRule type="expression" dxfId="258" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="314" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B52 A47">
-    <cfRule type="expression" dxfId="257" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="313" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B67">
-    <cfRule type="expression" dxfId="256" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="312" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B63">
-    <cfRule type="expression" dxfId="255" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="311" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C63">
-    <cfRule type="expression" dxfId="254" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="310" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C67">
-    <cfRule type="expression" dxfId="253" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="309" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46">
-    <cfRule type="expression" dxfId="252" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="308" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B78">
-    <cfRule type="expression" dxfId="251" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="307" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C74">
-    <cfRule type="expression" dxfId="250" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="306" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C78">
-    <cfRule type="expression" dxfId="249" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="305" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69:B74">
-    <cfRule type="expression" dxfId="248" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="304" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="247" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="303" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="246" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="302" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="expression" dxfId="245" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="301" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="expression" dxfId="244" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="300" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="243" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="299" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="242" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="298" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4974,137 +5430,137 @@
     <mergeCell ref="A58:B58"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A31:C35 A15:C21 A23:C29">
-    <cfRule type="expression" dxfId="241" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="297" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="expression" dxfId="240" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="296" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B46">
-    <cfRule type="expression" dxfId="239" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="295" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="expression" dxfId="238" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="294" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:C34">
-    <cfRule type="expression" dxfId="237" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="293" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C42">
-    <cfRule type="expression" dxfId="236" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="292" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B34">
-    <cfRule type="expression" dxfId="235" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="291" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B42">
-    <cfRule type="expression" dxfId="234" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="290" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C53">
-    <cfRule type="expression" dxfId="233" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="289" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:C57">
-    <cfRule type="expression" dxfId="232" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="288" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B57 A48">
-    <cfRule type="expression" dxfId="231" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="287" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B53 A48">
-    <cfRule type="expression" dxfId="230" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="286" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B68">
-    <cfRule type="expression" dxfId="229" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="285" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B64">
-    <cfRule type="expression" dxfId="228" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="284" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C64">
-    <cfRule type="expression" dxfId="227" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="283" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C68">
-    <cfRule type="expression" dxfId="226" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="282" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47">
-    <cfRule type="expression" dxfId="225" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="281" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B79">
-    <cfRule type="expression" dxfId="224" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="280" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C75">
-    <cfRule type="expression" dxfId="223" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="279" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C79">
-    <cfRule type="expression" dxfId="222" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="278" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70:B75">
-    <cfRule type="expression" dxfId="221" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="277" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="expression" dxfId="220" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="276" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="expression" dxfId="219" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="275" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58">
-    <cfRule type="expression" dxfId="218" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="274" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="expression" dxfId="217" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="273" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="216" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="272" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="215" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="271" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5855,117 +6311,117 @@
     <mergeCell ref="A56:B56"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A33:C37 A15:C22 A39:C44 A24:C31">
-    <cfRule type="expression" dxfId="214" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="270" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="expression" dxfId="213" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="269" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:C36">
-    <cfRule type="expression" dxfId="212" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="268" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B36">
-    <cfRule type="expression" dxfId="211" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="267" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C51">
-    <cfRule type="expression" dxfId="210" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="266" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C55">
-    <cfRule type="expression" dxfId="209" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="265" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B55 A46">
-    <cfRule type="expression" dxfId="208" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="264" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B51 A46">
-    <cfRule type="expression" dxfId="207" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="263" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B66">
-    <cfRule type="expression" dxfId="206" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="262" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B62">
-    <cfRule type="expression" dxfId="205" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="261" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C62">
-    <cfRule type="expression" dxfId="204" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="260" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C66">
-    <cfRule type="expression" dxfId="203" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="259" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="expression" dxfId="202" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="258" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:B77">
-    <cfRule type="expression" dxfId="201" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="257" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C73">
-    <cfRule type="expression" dxfId="200" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="256" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C77">
-    <cfRule type="expression" dxfId="199" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="255" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:B73">
-    <cfRule type="expression" dxfId="198" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="254" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="expression" dxfId="197" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="253" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="expression" dxfId="196" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="252" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" dxfId="195" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="251" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="expression" dxfId="194" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="250" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="193" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="249" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="expression" dxfId="192" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="248" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6646,137 +7102,137 @@
     <mergeCell ref="A49:B49"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A34:C34 A41:C41 A19:C20 A28:C28 A48:C48 A54:C55 A62:C63">
-    <cfRule type="expression" dxfId="191" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="247" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="expression" dxfId="190" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="246" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="expression" dxfId="189" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="245" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="expression" dxfId="188" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="244" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="expression" dxfId="187" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="243" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="expression" dxfId="186" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="242" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56">
-    <cfRule type="expression" dxfId="185" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="241" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="expression" dxfId="184" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="240" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:C40">
-    <cfRule type="expression" dxfId="183" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="239" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:C18">
-    <cfRule type="expression" dxfId="182" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="238" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:C27">
-    <cfRule type="expression" dxfId="181" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="237" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:C33">
-    <cfRule type="expression" dxfId="180" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="236" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="179" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="235" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C47">
-    <cfRule type="expression" dxfId="178" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="234" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C47">
-    <cfRule type="expression" dxfId="177" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="233" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43 A44:B47">
-    <cfRule type="expression" dxfId="176" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="232" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43 A44:B47">
-    <cfRule type="expression" dxfId="175" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="231" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="174" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="230" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="173" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="229" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B53">
-    <cfRule type="expression" dxfId="172" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="228" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B53">
-    <cfRule type="expression" dxfId="171" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="227" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C53">
-    <cfRule type="expression" dxfId="170" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="226" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C53">
-    <cfRule type="expression" dxfId="169" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="225" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B61">
-    <cfRule type="expression" dxfId="168" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="224" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C61">
-    <cfRule type="expression" dxfId="167" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="223" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:C61">
-    <cfRule type="expression" dxfId="166" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="222" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B61">
-    <cfRule type="expression" dxfId="165" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="221" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7507,192 +7963,192 @@
     <mergeCell ref="A59:B59"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A40:C40 A20:C25 A33:C33 A58:C58 A64:C65 A72:C73 A42:C50">
-    <cfRule type="expression" dxfId="164" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="220" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="expression" dxfId="163" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="219" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51">
-    <cfRule type="expression" dxfId="162" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="218" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34">
-    <cfRule type="expression" dxfId="161" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="217" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41">
-    <cfRule type="expression" dxfId="160" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="216" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="expression" dxfId="159" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="215" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="expression" dxfId="158" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C39">
-    <cfRule type="expression" dxfId="157" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:C19">
-    <cfRule type="expression" dxfId="156" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:C32">
-    <cfRule type="expression" dxfId="155" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="211" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:C39">
-    <cfRule type="expression" dxfId="154" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="210" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:B39">
-    <cfRule type="expression" dxfId="153" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="209" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C55 C57">
-    <cfRule type="expression" dxfId="152" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="208" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C55 C57">
-    <cfRule type="expression" dxfId="151" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="207" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52 A53:B55 A57:B57">
-    <cfRule type="expression" dxfId="150" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="206" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52 A53:B55 A57:B57">
-    <cfRule type="expression" dxfId="149" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="205" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="148" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="204" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="147" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B63">
-    <cfRule type="expression" dxfId="146" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B63">
-    <cfRule type="expression" dxfId="145" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:C63">
-    <cfRule type="expression" dxfId="144" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="200" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:C63">
-    <cfRule type="expression" dxfId="143" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:B71">
-    <cfRule type="expression" dxfId="142" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C71">
-    <cfRule type="expression" dxfId="141" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="197" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C71">
-    <cfRule type="expression" dxfId="140" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="196" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:B71">
-    <cfRule type="expression" dxfId="139" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="195" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="138" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="194" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="expression" dxfId="137" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="193" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B56">
-    <cfRule type="expression" dxfId="136" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="192" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B56">
-    <cfRule type="expression" dxfId="135" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="191" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="134" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="190" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="133" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="189" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B60">
-    <cfRule type="expression" dxfId="132" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B60">
-    <cfRule type="expression" dxfId="131" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="130" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="129" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:B67">
-    <cfRule type="expression" dxfId="128" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67:B67">
-    <cfRule type="expression" dxfId="127" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8329,307 +8785,307 @@
     <mergeCell ref="A57:B57"/>
   </mergeCells>
   <conditionalFormatting sqref="A14 A39:C39 A32:C32 A56:C56 A62:C63 A70:C71 A42:C42 A16:C24 A44:C44 A46:C48">
-    <cfRule type="expression" dxfId="126" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="64" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="125" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="63" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="expression" dxfId="124" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="60" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="expression" dxfId="123" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="62" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="122" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="61" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="expression" dxfId="121" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="59" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="expression" dxfId="120" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="58" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C38">
-    <cfRule type="expression" dxfId="119" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="53" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:C31">
-    <cfRule type="expression" dxfId="118" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="56" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:C38">
-    <cfRule type="expression" dxfId="117" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="55" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:B38">
-    <cfRule type="expression" dxfId="116" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="54" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C51 C55 C53">
-    <cfRule type="expression" dxfId="115" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="49" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:C51 C55 C53">
-    <cfRule type="expression" dxfId="114" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="50" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50 A51:B51 A55:B55 A53:B53">
-    <cfRule type="expression" dxfId="113" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="52" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50 A51:B51 A55:B55 A53:B53">
-    <cfRule type="expression" dxfId="112" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="51" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B61">
-    <cfRule type="expression" dxfId="111" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="46" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B61">
-    <cfRule type="expression" dxfId="110" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="45" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C61">
-    <cfRule type="expression" dxfId="109" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="43" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:C61">
-    <cfRule type="expression" dxfId="108" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="44" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66:B69">
-    <cfRule type="expression" dxfId="107" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C69">
-    <cfRule type="expression" dxfId="106" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="39" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C69">
-    <cfRule type="expression" dxfId="105" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="40" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66:B69">
-    <cfRule type="expression" dxfId="104" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="41" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="103" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="35" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="102" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="36" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:B54">
-    <cfRule type="expression" dxfId="101" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="38" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:B54">
-    <cfRule type="expression" dxfId="100" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="37" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="99" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="31" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="98" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="32" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B58">
-    <cfRule type="expression" dxfId="97" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="34" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B58">
-    <cfRule type="expression" dxfId="96" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="33" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="95" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="94" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="28" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:B65">
-    <cfRule type="expression" dxfId="93" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="30" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:B65">
-    <cfRule type="expression" dxfId="92" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="29" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="91" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="90" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B15">
-    <cfRule type="expression" dxfId="89" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15:B15">
-    <cfRule type="expression" dxfId="88" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:C26">
-    <cfRule type="expression" dxfId="87" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="22" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:C27">
-    <cfRule type="expression" dxfId="86" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="21" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:C29">
-    <cfRule type="expression" dxfId="85" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="20" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:C28">
-    <cfRule type="expression" dxfId="84" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="19" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:C30">
-    <cfRule type="expression" dxfId="83" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="18" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="82" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="15" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:C41">
-    <cfRule type="expression" dxfId="81" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="17" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:B41">
-    <cfRule type="expression" dxfId="80" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="16" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="79" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="12" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:C43">
-    <cfRule type="expression" dxfId="78" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="14" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:B43">
-    <cfRule type="expression" dxfId="77" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="76" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:C45">
-    <cfRule type="expression" dxfId="75" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="11" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:B45">
-    <cfRule type="expression" dxfId="74" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="10" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="expression" dxfId="73" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="8" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="expression" dxfId="72" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="7" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="71" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="3" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="70" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="4" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="expression" dxfId="69" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="6" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="expression" dxfId="68" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="5" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="67" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="66" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8645,10 +9101,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -8752,7 +9208,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>17</v>
@@ -8774,7 +9230,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>17</v>
@@ -8832,7 +9288,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>17</v>
@@ -8854,7 +9310,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>17</v>
@@ -8865,7 +9321,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>33</v>
@@ -8876,7 +9332,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>17</v>
@@ -8909,7 +9365,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34" s="25" t="s">
         <v>17</v>
@@ -8931,7 +9387,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B36" s="25" t="s">
         <v>17</v>
@@ -9017,7 +9473,7 @@
         <v>106</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C44" s="25">
         <v>2</v>
@@ -9039,7 +9495,7 @@
         <v>106</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C46" s="25">
         <v>2</v>
@@ -9068,34 +9524,70 @@
       <c r="C49" s="31"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="18"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
+      <c r="A50" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="18"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
+      <c r="A51" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="18"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
+      <c r="A52" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="18"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
+      <c r="A53" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="25">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
+      <c r="A54" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="18"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
+      <c r="A55" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="20"/>
@@ -9103,7 +9595,7 @@
       <c r="C56" s="27"/>
       <c r="D56">
         <f>SUM(C50:C56)</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -9115,149 +9607,273 @@
       <c r="C57" s="31"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="18"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
+      <c r="A58" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="25">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="18"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
+      <c r="A59" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="25">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+      <c r="A60" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="18"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
+      <c r="A61" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="25">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="20"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-    </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="20"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
-      <c r="D63">
-        <f>SUM(C58:C63)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="35">
-        <f>A57+1</f>
-        <v>44367</v>
-      </c>
-      <c r="B64" s="36"/>
-      <c r="C64" s="31"/>
+      <c r="A62" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="26">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="26">
+        <v>2</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="18"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
+      <c r="A65" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="26">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
+      <c r="A66" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66" s="26">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
+      <c r="A67" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B67" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" s="26">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="18"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
+      <c r="A68" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" s="26">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="18"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
+      <c r="A69" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="26">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="20"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="27"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="37"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="26"/>
+      <c r="D70">
+        <f>SUM(C58:C71)</f>
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="20"/>
       <c r="B71" s="27"/>
       <c r="C71" s="27"/>
-      <c r="D71">
-        <f>SUM(C65:C71)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="21"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="35">
+        <f>A57+1</f>
+        <v>44367</v>
+      </c>
+      <c r="B72" s="36"/>
+      <c r="C72" s="31"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="10"/>
-      <c r="B73" s="28"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="12"/>
-    </row>
-    <row r="74" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="17" t="s">
+      <c r="A73" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C73" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C74" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="18"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="18"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="18"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="20"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="27"/>
+      <c r="D78">
+        <f>SUM(C73:C79)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="20"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="12"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="10"/>
+      <c r="B81" s="28"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="13"/>
+    </row>
+    <row r="82" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B74" s="17"/>
-      <c r="C74" s="32">
-        <f>SUM(C14:C71)</f>
-        <v>33.25</v>
-      </c>
-      <c r="D74" s="13"/>
-    </row>
-    <row r="75" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="9"/>
-      <c r="B75" s="29"/>
-      <c r="C75" s="29"/>
-    </row>
-    <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A76" s="10" t="s">
+      <c r="B82" s="17"/>
+      <c r="C82" s="32">
+        <f>SUM(C14:C79)</f>
+        <v>60.25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="18.75" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="9"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="11"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="28"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="11"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="22"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="30"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="22"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="30"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="9"/>
-      <c r="B79" s="29"/>
-      <c r="C79" s="29"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="23"/>
-      <c r="B80" s="23"/>
-      <c r="C80" s="23"/>
-    </row>
-    <row r="82" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
+      <c r="B84" s="28"/>
+      <c r="C84" s="28"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="22"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="22"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="30"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="9"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="23"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+    </row>
+    <row r="90" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A72:B72"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A33:B33"/>
@@ -9265,317 +9881,592 @@
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A57:B57"/>
   </mergeCells>
-  <conditionalFormatting sqref="A14 A39:C39 A32:C32 A56:C56 A62:C63 A70:C71 A42:C42 A16:C16 A44:C44 A46:C48 A18:C24 C17">
-    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
+  <conditionalFormatting sqref="A14 A39:C39 A32:C32 A56:C56 A71:C71 A78:C79 A42:C42 A16:C16 A44:C44 A46:C48 A18:C24 C17 C62:C64 C70">
+    <cfRule type="expression" dxfId="121" priority="131" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="expression" dxfId="64" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="130" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="expression" dxfId="63" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="127" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="expression" dxfId="62" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="129" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="61" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="128" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="expression" dxfId="60" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="126" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A72">
+    <cfRule type="expression" dxfId="115" priority="125" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:C38">
+    <cfRule type="expression" dxfId="114" priority="121" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:C31">
+    <cfRule type="expression" dxfId="113" priority="124" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:C38">
+    <cfRule type="expression" dxfId="112" priority="123" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:B38">
+    <cfRule type="expression" dxfId="111" priority="122" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:C51 C55 C53">
+    <cfRule type="expression" dxfId="110" priority="117" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50:C51 C55 C53">
+    <cfRule type="expression" dxfId="109" priority="118" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50 A51:B51 A53:B53">
+    <cfRule type="expression" dxfId="108" priority="120" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50 A51:B51 A53:B53">
+    <cfRule type="expression" dxfId="107" priority="119" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:B59 A61:B61">
+    <cfRule type="expression" dxfId="106" priority="116" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59:B59 A61:B61">
+    <cfRule type="expression" dxfId="105" priority="115" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:C61">
+    <cfRule type="expression" dxfId="104" priority="113" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:C61">
+    <cfRule type="expression" dxfId="103" priority="114" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75:B77">
+    <cfRule type="expression" dxfId="102" priority="112" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C75:C77">
+    <cfRule type="expression" dxfId="101" priority="109" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C75:C77">
+    <cfRule type="expression" dxfId="100" priority="110" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A75:B77">
+    <cfRule type="expression" dxfId="99" priority="111" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="98" priority="105" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="expression" dxfId="97" priority="106" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B54">
+    <cfRule type="expression" dxfId="96" priority="108" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B54">
+    <cfRule type="expression" dxfId="95" priority="107" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="94" priority="101" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="93" priority="102" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="92" priority="94" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="91" priority="93" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="expression" dxfId="86" priority="85" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:B41">
+    <cfRule type="expression" dxfId="85" priority="86" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="expression" dxfId="84" priority="96" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="expression" dxfId="83" priority="95" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:C26">
+    <cfRule type="expression" dxfId="82" priority="92" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:C27">
+    <cfRule type="expression" dxfId="81" priority="91" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:C29">
+    <cfRule type="expression" dxfId="80" priority="90" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:C28">
+    <cfRule type="expression" dxfId="79" priority="89" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:C30">
+    <cfRule type="expression" dxfId="78" priority="88" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:C41">
+    <cfRule type="expression" dxfId="77" priority="87" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" dxfId="76" priority="79" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:C45">
+    <cfRule type="expression" dxfId="75" priority="81" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:B45">
+    <cfRule type="expression" dxfId="74" priority="80" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="73" priority="78" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B50">
+    <cfRule type="expression" dxfId="72" priority="77" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="71" priority="73" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="expression" dxfId="70" priority="74" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="expression" dxfId="69" priority="56" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="expression" dxfId="68" priority="55" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="expression" dxfId="67" priority="54" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="expression" dxfId="66" priority="53" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:C43">
+    <cfRule type="expression" dxfId="65" priority="70" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="expression" dxfId="64" priority="69" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17">
+    <cfRule type="expression" dxfId="63" priority="68" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="expression" dxfId="62" priority="67" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="expression" dxfId="61" priority="66" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="expression" dxfId="60" priority="65" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52">
+    <cfRule type="expression" dxfId="59" priority="64" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="58" priority="63" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52">
+    <cfRule type="expression" dxfId="57" priority="62" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="expression" dxfId="56" priority="61" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="expression" dxfId="55" priority="60" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55">
+    <cfRule type="expression" dxfId="54" priority="59" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55">
+    <cfRule type="expression" dxfId="53" priority="58" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="expression" dxfId="52" priority="57" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62 A70">
+    <cfRule type="expression" dxfId="51" priority="48" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62 B70">
+    <cfRule type="expression" dxfId="50" priority="47" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62 B70">
+    <cfRule type="expression" dxfId="49" priority="46" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63">
+    <cfRule type="expression" dxfId="48" priority="45" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60">
+    <cfRule type="expression" dxfId="47" priority="52" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60">
+    <cfRule type="expression" dxfId="46" priority="51" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60">
+    <cfRule type="expression" dxfId="45" priority="50" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62 A70">
+    <cfRule type="expression" dxfId="44" priority="49" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64">
+    <cfRule type="expression" dxfId="43" priority="38" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="42" priority="37" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="expression" dxfId="41" priority="36" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="expression" dxfId="40" priority="35" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63">
+    <cfRule type="expression" dxfId="39" priority="44" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B63">
+    <cfRule type="expression" dxfId="38" priority="43" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B63">
+    <cfRule type="expression" dxfId="37" priority="42" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="expression" dxfId="59" priority="60" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C38">
-    <cfRule type="expression" dxfId="58" priority="56" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31:C31">
-    <cfRule type="expression" dxfId="57" priority="59" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34:C38">
-    <cfRule type="expression" dxfId="56" priority="58" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34:B38">
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50:C51 C55 C53">
-    <cfRule type="expression" dxfId="54" priority="52" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50:C51 C55 C53">
-    <cfRule type="expression" dxfId="53" priority="53" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50 A51:B51 A55:B55 A53:B53">
-    <cfRule type="expression" dxfId="52" priority="55" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50 A51:B51 A55:B55 A53:B53">
-    <cfRule type="expression" dxfId="51" priority="54" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:B61">
-    <cfRule type="expression" dxfId="50" priority="51" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:B61">
-    <cfRule type="expression" dxfId="49" priority="50" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C61">
-    <cfRule type="expression" dxfId="48" priority="48" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C61">
-    <cfRule type="expression" dxfId="47" priority="49" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66:B69">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66:C69">
-    <cfRule type="expression" dxfId="45" priority="44" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66:C69">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66:B69">
-    <cfRule type="expression" dxfId="43" priority="46" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="42" priority="40" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="expression" dxfId="41" priority="41" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:B54">
-    <cfRule type="expression" dxfId="40" priority="43" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:B54">
-    <cfRule type="expression" dxfId="39" priority="42" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="38" priority="36" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="37" priority="37" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58:B58">
-    <cfRule type="expression" dxfId="36" priority="39" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58:B58">
-    <cfRule type="expression" dxfId="35" priority="38" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="34" priority="32" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="33" priority="33" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:B65">
-    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:B65">
-    <cfRule type="expression" dxfId="31" priority="34" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="30" priority="28" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="28" priority="31" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="expression" dxfId="27" priority="30" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26:C26">
+    <cfRule type="expression" dxfId="36" priority="41" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64">
+    <cfRule type="expression" dxfId="35" priority="40" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64">
+    <cfRule type="expression" dxfId="34" priority="39" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65">
+    <cfRule type="expression" dxfId="33" priority="34" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65">
+    <cfRule type="expression" dxfId="32" priority="33" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="31" priority="32" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="expression" dxfId="30" priority="31" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66">
+    <cfRule type="expression" dxfId="28" priority="29" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66">
+    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67">
     <cfRule type="expression" dxfId="26" priority="27" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:C27">
+  <conditionalFormatting sqref="A67">
     <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29:C29">
+  <conditionalFormatting sqref="A67">
     <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28:C28">
+  <conditionalFormatting sqref="B67">
     <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30:C30">
+  <conditionalFormatting sqref="B67">
     <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="21" priority="20" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:C41">
-    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A41:B41">
-    <cfRule type="expression" dxfId="19" priority="21" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="15" priority="14" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:C45">
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:B45">
-    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
+  <conditionalFormatting sqref="C68">
+    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="expression" dxfId="20" priority="21" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B68">
+    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B68">
+    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C69">
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69">
     <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C73">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
     <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52">
-    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A43:C43">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
+  <conditionalFormatting sqref="B73">
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B73">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74">
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A74">
+    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
+  <conditionalFormatting sqref="B74">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>